<commit_message>
Archivos actualizados hasta J5
</commit_message>
<xml_diff>
--- a/CSV obtenidos/J1_heatmaps_jugadores.xlsx
+++ b/CSV obtenidos/J1_heatmaps_jugadores.xlsx
@@ -8,19 +8,19 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sebastián Rodríguez" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cecilio Waterman" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Juan Freytes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jiovany Ramos" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Renzo Garces" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hernán Barcos" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Juan Freytes" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kevin Serna" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cecilio Waterman" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hernán Barcos" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jiovany Ramos" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Catriel Cabellos" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kevin Serna" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aldair Fuentes" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jesús Castillo" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Saravia" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ricardo Lagos" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Zanelatto" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Adrián Arregui" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Renzo Garces" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Adrián Arregui" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aldair Fuentes" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Zanelatto" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jesús Castillo" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Saravia" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ricardo Lagos" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -781,6 +781,708 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B2" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B3" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>52</v>
+      </c>
+      <c r="B4" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B5" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B6" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>34</v>
+      </c>
+      <c r="B8" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>53</v>
+      </c>
+      <c r="B9" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>88</v>
+      </c>
+      <c r="B10" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>29</v>
+      </c>
+      <c r="B12" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>34</v>
+      </c>
+      <c r="B13" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>28</v>
+      </c>
+      <c r="B14" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>26</v>
+      </c>
+      <c r="B15" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>21</v>
+      </c>
+      <c r="B16" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>41</v>
+      </c>
+      <c r="B17" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>27</v>
+      </c>
+      <c r="B18" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>25</v>
+      </c>
+      <c r="B19" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>24</v>
+      </c>
+      <c r="B20" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>39</v>
+      </c>
+      <c r="B23" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>35</v>
+      </c>
+      <c r="B24" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>53</v>
+      </c>
+      <c r="B25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>41</v>
+      </c>
+      <c r="B26" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>42</v>
+      </c>
+      <c r="B27" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>35</v>
+      </c>
+      <c r="B28" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>35</v>
+      </c>
+      <c r="B29" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>21</v>
+      </c>
+      <c r="B30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>24</v>
+      </c>
+      <c r="B31" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>34</v>
+      </c>
+      <c r="B32" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>35</v>
+      </c>
+      <c r="B33" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>31</v>
+      </c>
+      <c r="B34" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>29</v>
+      </c>
+      <c r="B35" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>11</v>
+      </c>
+      <c r="B36" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>39</v>
+      </c>
+      <c r="B37" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>43</v>
+      </c>
+      <c r="B38" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>43</v>
+      </c>
+      <c r="B39" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>15</v>
+      </c>
+      <c r="B40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>15</v>
+      </c>
+      <c r="B41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>34</v>
+      </c>
+      <c r="B42" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>35</v>
+      </c>
+      <c r="B43" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>54</v>
+      </c>
+      <c r="B46" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>35</v>
+      </c>
+      <c r="B48" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>39</v>
+      </c>
+      <c r="B49" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>36</v>
+      </c>
+      <c r="B50" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>15</v>
+      </c>
+      <c r="B51" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>26</v>
+      </c>
+      <c r="B52" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>27</v>
+      </c>
+      <c r="B53" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>27</v>
+      </c>
+      <c r="B54" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>74</v>
+      </c>
+      <c r="B55" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>10</v>
+      </c>
+      <c r="B56" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3</v>
+      </c>
+      <c r="B57" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>39</v>
+      </c>
+      <c r="B58" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>13</v>
+      </c>
+      <c r="B59" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>30</v>
+      </c>
+      <c r="B60" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>10</v>
+      </c>
+      <c r="B61" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>5</v>
+      </c>
+      <c r="B62" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2</v>
+      </c>
+      <c r="B63" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>25</v>
+      </c>
+      <c r="B65" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>25</v>
+      </c>
+      <c r="B66" t="n">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B2" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B3" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33</v>
+      </c>
+      <c r="B4" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>72</v>
+      </c>
+      <c r="B5" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B6" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>45</v>
+      </c>
+      <c r="B7" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>43</v>
+      </c>
+      <c r="B8" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>52</v>
+      </c>
+      <c r="B9" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>43</v>
+      </c>
+      <c r="B10" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>29</v>
+      </c>
+      <c r="B11" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>29</v>
+      </c>
+      <c r="B12" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>43</v>
+      </c>
+      <c r="B13" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>40</v>
+      </c>
+      <c r="B14" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>93</v>
+      </c>
+      <c r="B15" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>96</v>
+      </c>
+      <c r="B16" t="n">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -870,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1109,7 +1811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1444,13 +2146,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1472,122 +2174,490 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B2" t="n">
-        <v>62</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="B3" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B6" t="n">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B7" t="n">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="B8" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B9" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B10" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="n">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B15" t="n">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>30</v>
+      </c>
+      <c r="B16" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>43</v>
+      </c>
+      <c r="B17" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>95</v>
+      </c>
+      <c r="B18" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>26</v>
+      </c>
+      <c r="B19" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>53</v>
+      </c>
+      <c r="B20" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>88</v>
+      </c>
+      <c r="B21" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>86</v>
+      </c>
+      <c r="B22" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>67</v>
+      </c>
+      <c r="B23" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>9</v>
+      </c>
+      <c r="B24" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>46</v>
+      </c>
+      <c r="B25" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>53</v>
+      </c>
+      <c r="B26" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>24</v>
+      </c>
+      <c r="B27" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>48</v>
+      </c>
+      <c r="B28" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>51</v>
+      </c>
+      <c r="B29" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>36</v>
+      </c>
+      <c r="B30" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>13</v>
+      </c>
+      <c r="B31" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>15</v>
+      </c>
+      <c r="B32" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>51</v>
+      </c>
+      <c r="B33" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>63</v>
+      </c>
+      <c r="B34" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>27</v>
+      </c>
+      <c r="B35" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>56</v>
+      </c>
+      <c r="B36" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>60</v>
+      </c>
+      <c r="B37" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>60</v>
+      </c>
+      <c r="B38" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>46</v>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>38</v>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>28</v>
+      </c>
+      <c r="B42" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>20</v>
+      </c>
+      <c r="B43" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>53</v>
+      </c>
+      <c r="B44" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>65</v>
+      </c>
+      <c r="B45" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>29</v>
+      </c>
+      <c r="B46" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>24</v>
+      </c>
+      <c r="B47" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>54</v>
+      </c>
+      <c r="B48" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>54</v>
+      </c>
+      <c r="B49" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>54</v>
+      </c>
+      <c r="B50" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>25</v>
+      </c>
+      <c r="B51" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>15</v>
+      </c>
+      <c r="B52" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>15</v>
+      </c>
+      <c r="B53" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32</v>
+      </c>
+      <c r="B54" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>25</v>
+      </c>
+      <c r="B55" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>5</v>
+      </c>
+      <c r="B56" t="n">
         <v>96</v>
       </c>
-      <c r="B16" t="n">
-        <v>97</v>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>5</v>
+      </c>
+      <c r="B57" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>7</v>
+      </c>
+      <c r="B58" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>9</v>
+      </c>
+      <c r="B59" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>11</v>
+      </c>
+      <c r="B60" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B61" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1</v>
+      </c>
+      <c r="B62" t="n">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1595,13 +2665,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1623,183 +2693,183 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B3" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="B7" t="n">
-        <v>68</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B8" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B11" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B12" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B13" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B14" t="n">
-        <v>74</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B16" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B17" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B18" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B21" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B22" t="n">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" t="n">
         <v>23</v>
@@ -1807,218 +2877,378 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B25" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B26" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B27" t="n">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B28" t="n">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B29" t="n">
-        <v>58</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B30" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B31" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B32" t="n">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B33" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B34" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B35" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B37" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B38" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B39" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B41" t="n">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="B42" t="n">
-        <v>93</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B43" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B44" t="n">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B45" t="n">
-        <v>91</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B46" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B48" t="n">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B49" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>70</v>
+      </c>
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>55</v>
+      </c>
+      <c r="B52" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>30</v>
+      </c>
+      <c r="B53" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>56</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>57</v>
+      </c>
+      <c r="B55" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>57</v>
+      </c>
+      <c r="B56" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>92</v>
+      </c>
+      <c r="B57" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>96</v>
+      </c>
+      <c r="B58" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>76</v>
+      </c>
+      <c r="B59" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>76</v>
+      </c>
+      <c r="B60" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>73</v>
+      </c>
+      <c r="B61" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>58</v>
+      </c>
+      <c r="B62" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>55</v>
+      </c>
+      <c r="B63" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
         <v>28</v>
       </c>
-      <c r="B51" t="n">
-        <v>29</v>
+      <c r="B64" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>27</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30</v>
+      </c>
+      <c r="B66" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>12</v>
+      </c>
+      <c r="B67" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>12</v>
+      </c>
+      <c r="B68" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>84</v>
+      </c>
+      <c r="B69" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>47</v>
+      </c>
+      <c r="B70" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>9</v>
+      </c>
+      <c r="B71" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +3256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2249,13 +3479,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2277,282 +3507,282 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B2" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B3" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B4" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B5" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B7" t="n">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B8" t="n">
-        <v>81</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B9" t="n">
-        <v>100</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B10" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B11" t="n">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B12" t="n">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B14" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B15" t="n">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B17" t="n">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B18" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>89</v>
+      </c>
+      <c r="B20" t="n">
         <v>53</v>
-      </c>
-      <c r="B20" t="n">
-        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B22" t="n">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B23" t="n">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B24" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B25" t="n">
-        <v>73</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B26" t="n">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B27" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B29" t="n">
-        <v>83</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B30" t="n">
-        <v>71</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B31" t="n">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B32" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B33" t="n">
-        <v>67</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B35" t="n">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>77</v>
+      </c>
+      <c r="B36" t="n">
         <v>56</v>
-      </c>
-      <c r="B36" t="n">
-        <v>78</v>
       </c>
     </row>
     <row r="37">
@@ -2560,207 +3790,175 @@
         <v>60</v>
       </c>
       <c r="B37" t="n">
-        <v>91</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B38" t="n">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="B41" t="n">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B42" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B44" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B45" t="n">
-        <v>65</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B46" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B47" t="n">
-        <v>67</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B48" t="n">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B49" t="n">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B50" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B51" t="n">
-        <v>73</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B52" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B53" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B54" t="n">
-        <v>92</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="B55" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B56" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="B57" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="B58" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>9</v>
-      </c>
-      <c r="B59" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>11</v>
-      </c>
-      <c r="B60" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B61" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>1</v>
-      </c>
-      <c r="B62" t="n">
-        <v>92</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2768,7 +3966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3496,532 +4694,6 @@
       </c>
       <c r="B89" t="n">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B2" t="n">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B58"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>49</v>
-      </c>
-      <c r="B2" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>60</v>
-      </c>
-      <c r="B3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>59</v>
-      </c>
-      <c r="B4" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>60</v>
-      </c>
-      <c r="B5" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>34</v>
-      </c>
-      <c r="B6" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>36</v>
-      </c>
-      <c r="B7" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>65</v>
-      </c>
-      <c r="B8" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>70</v>
-      </c>
-      <c r="B9" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>87</v>
-      </c>
-      <c r="B10" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>44</v>
-      </c>
-      <c r="B11" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>42</v>
-      </c>
-      <c r="B12" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>30</v>
-      </c>
-      <c r="B13" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>50</v>
-      </c>
-      <c r="B14" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>44</v>
-      </c>
-      <c r="B15" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>75</v>
-      </c>
-      <c r="B16" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>83</v>
-      </c>
-      <c r="B17" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>84</v>
-      </c>
-      <c r="B18" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>89</v>
-      </c>
-      <c r="B19" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>89</v>
-      </c>
-      <c r="B20" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>87</v>
-      </c>
-      <c r="B21" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>88</v>
-      </c>
-      <c r="B22" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>82</v>
-      </c>
-      <c r="B23" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>60</v>
-      </c>
-      <c r="B24" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>60</v>
-      </c>
-      <c r="B25" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>69</v>
-      </c>
-      <c r="B26" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>46</v>
-      </c>
-      <c r="B27" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>33</v>
-      </c>
-      <c r="B28" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>77</v>
-      </c>
-      <c r="B29" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>71</v>
-      </c>
-      <c r="B30" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>43</v>
-      </c>
-      <c r="B31" t="n">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>61</v>
-      </c>
-      <c r="B32" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>68</v>
-      </c>
-      <c r="B33" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>39</v>
-      </c>
-      <c r="B34" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>79</v>
-      </c>
-      <c r="B35" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>77</v>
-      </c>
-      <c r="B36" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>60</v>
-      </c>
-      <c r="B37" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>56</v>
-      </c>
-      <c r="B38" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>45</v>
-      </c>
-      <c r="B39" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>45</v>
-      </c>
-      <c r="B40" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>89</v>
-      </c>
-      <c r="B41" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>5</v>
-      </c>
-      <c r="B42" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>48</v>
-      </c>
-      <c r="B43" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>47</v>
-      </c>
-      <c r="B44" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>41</v>
-      </c>
-      <c r="B45" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>41</v>
-      </c>
-      <c r="B46" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>58</v>
-      </c>
-      <c r="B47" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>88</v>
-      </c>
-      <c r="B48" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>61</v>
-      </c>
-      <c r="B49" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>42</v>
-      </c>
-      <c r="B50" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>28</v>
-      </c>
-      <c r="B51" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>44</v>
-      </c>
-      <c r="B52" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>64</v>
-      </c>
-      <c r="B53" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>66</v>
-      </c>
-      <c r="B54" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>64</v>
-      </c>
-      <c r="B55" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>50</v>
-      </c>
-      <c r="B56" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>97</v>
-      </c>
-      <c r="B57" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>95</v>
-      </c>
-      <c r="B58" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4586,7 +5258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4608,562 +5280,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>95</v>
-      </c>
-      <c r="B3" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>62</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>63</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>91</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>45</v>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>65</v>
-      </c>
-      <c r="B8" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>32</v>
-      </c>
-      <c r="B9" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>46</v>
-      </c>
-      <c r="B10" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>54</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>62</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>56</v>
-      </c>
-      <c r="B13" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>70</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>70</v>
-      </c>
-      <c r="B15" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>63</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>64</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>68</v>
-      </c>
-      <c r="B18" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>63</v>
-      </c>
-      <c r="B19" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>83</v>
-      </c>
-      <c r="B20" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>85</v>
-      </c>
-      <c r="B21" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>85</v>
-      </c>
-      <c r="B22" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>59</v>
-      </c>
-      <c r="B23" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>59</v>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>58</v>
-      </c>
-      <c r="B25" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>50</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>53</v>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>53</v>
-      </c>
-      <c r="B28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>86</v>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>73</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>74</v>
-      </c>
-      <c r="B31" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>74</v>
-      </c>
-      <c r="B32" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>89</v>
-      </c>
-      <c r="B33" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>94</v>
-      </c>
-      <c r="B34" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>90</v>
-      </c>
-      <c r="B35" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>44</v>
-      </c>
-      <c r="B36" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>92</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>86</v>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>98</v>
-      </c>
-      <c r="B39" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>45</v>
-      </c>
-      <c r="B40" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>80</v>
-      </c>
-      <c r="B41" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>84</v>
-      </c>
-      <c r="B42" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>78</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>71</v>
-      </c>
-      <c r="B44" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>27</v>
-      </c>
-      <c r="B45" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>39</v>
-      </c>
-      <c r="B46" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>75</v>
-      </c>
-      <c r="B47" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>87</v>
-      </c>
-      <c r="B48" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>41</v>
-      </c>
-      <c r="B49" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>70</v>
-      </c>
-      <c r="B51" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>55</v>
-      </c>
-      <c r="B52" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>30</v>
-      </c>
-      <c r="B53" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>56</v>
-      </c>
-      <c r="B54" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>57</v>
-      </c>
-      <c r="B55" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>57</v>
-      </c>
-      <c r="B56" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>92</v>
-      </c>
-      <c r="B57" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>96</v>
-      </c>
-      <c r="B58" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>76</v>
-      </c>
-      <c r="B59" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>76</v>
-      </c>
-      <c r="B60" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>73</v>
-      </c>
-      <c r="B61" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>58</v>
-      </c>
-      <c r="B62" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>55</v>
-      </c>
-      <c r="B63" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>28</v>
-      </c>
-      <c r="B64" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>27</v>
-      </c>
-      <c r="B65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>30</v>
-      </c>
-      <c r="B66" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>12</v>
-      </c>
-      <c r="B67" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>12</v>
-      </c>
-      <c r="B68" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>84</v>
-      </c>
-      <c r="B69" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>47</v>
-      </c>
-      <c r="B70" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>9</v>
-      </c>
-      <c r="B71" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -5177,7 +5297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5199,522 +5319,402 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B3" t="n">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B5" t="n">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B7" t="n">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B9" t="n">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B10" t="n">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B12" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B13" t="n">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B14" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B15" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B16" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B17" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B18" t="n">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B19" t="n">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B20" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="B21" t="n">
-        <v>67</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B22" t="n">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B23" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B24" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="B26" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="B27" t="n">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B28" t="n">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B29" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B30" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B31" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B32" t="n">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B33" t="n">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B34" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B35" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B36" t="n">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B37" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B38" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B39" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B42" t="n">
-        <v>29</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B43" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B44" t="n">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B46" t="n">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B47" t="n">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B48" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B49" t="n">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B50" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B51" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>26</v>
-      </c>
-      <c r="B52" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>27</v>
-      </c>
-      <c r="B53" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>27</v>
-      </c>
-      <c r="B54" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>74</v>
-      </c>
-      <c r="B55" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>10</v>
-      </c>
-      <c r="B56" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>3</v>
-      </c>
-      <c r="B57" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>39</v>
-      </c>
-      <c r="B58" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>13</v>
-      </c>
-      <c r="B59" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>30</v>
-      </c>
-      <c r="B60" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>10</v>
-      </c>
-      <c r="B61" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>5</v>
-      </c>
-      <c r="B62" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>2</v>
-      </c>
-      <c r="B63" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>0</v>
-      </c>
-      <c r="B64" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>25</v>
-      </c>
-      <c r="B65" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>25</v>
-      </c>
-      <c r="B66" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
un par de cagadas al traer los datos de la J6
</commit_message>
<xml_diff>
--- a/CSV obtenidos/J1_heatmaps_jugadores.xlsx
+++ b/CSV obtenidos/J1_heatmaps_jugadores.xlsx
@@ -8,19 +8,19 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sebastián Rodríguez" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Juan Freytes" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kevin Serna" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hernán Barcos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Juan Freytes" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cecilio Waterman" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hernán Barcos" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jiovany Ramos" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Catriel Cabellos" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Renzo Garces" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Adrián Arregui" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kevin Serna" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Catriel Cabellos" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Renzo Garces" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Adrián Arregui" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jiovany Ramos" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aldair Fuentes" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Zanelatto" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jesús Castillo" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Saravia" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ricardo Lagos" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jesús Castillo" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Zanelatto" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ricardo Lagos" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Franco Saravia" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1332,6 +1332,101 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B2" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B4" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>55</v>
+      </c>
+      <c r="B5" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>31</v>
+      </c>
+      <c r="B7" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>34</v>
+      </c>
+      <c r="B8" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>17</v>
+      </c>
+      <c r="B9" t="n">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1477,13 +1572,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,66 +1600,306 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B2" t="n">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B3" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B4" t="n">
-        <v>92</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B5" t="n">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B7" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B9" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>64</v>
+      </c>
+      <c r="B10" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>37</v>
+      </c>
+      <c r="B11" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>60</v>
+      </c>
+      <c r="B12" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>44</v>
+      </c>
+      <c r="B13" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>44</v>
+      </c>
+      <c r="B14" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>70</v>
+      </c>
+      <c r="B15" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>97</v>
+      </c>
+      <c r="B16" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>99</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>99</v>
+      </c>
+      <c r="B18" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>75</v>
+      </c>
+      <c r="B19" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>70</v>
+      </c>
+      <c r="B20" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>40</v>
+      </c>
+      <c r="B21" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>37</v>
+      </c>
+      <c r="B22" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>37</v>
+      </c>
+      <c r="B23" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>46</v>
+      </c>
+      <c r="B24" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>79</v>
+      </c>
+      <c r="B25" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>66</v>
+      </c>
+      <c r="B26" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>97</v>
+      </c>
+      <c r="B27" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>68</v>
+      </c>
+      <c r="B28" t="n">
         <v>88</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>74</v>
+      </c>
+      <c r="B29" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>48</v>
+      </c>
+      <c r="B30" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>70</v>
+      </c>
+      <c r="B31" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>23</v>
+      </c>
+      <c r="B32" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>22</v>
+      </c>
+      <c r="B33" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>26</v>
+      </c>
+      <c r="B34" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>59</v>
+      </c>
+      <c r="B35" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>30</v>
+      </c>
+      <c r="B36" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>20</v>
+      </c>
+      <c r="B37" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>24</v>
+      </c>
+      <c r="B38" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>39</v>
+      </c>
+      <c r="B39" t="n">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1572,7 +1907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1811,13 +2146,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1839,263 +2174,263 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B2" t="n">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" t="n">
-        <v>81</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B4" t="n">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B5" t="n">
-        <v>65</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B7" t="n">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B8" t="n">
-        <v>86</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B9" t="n">
-        <v>96</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B10" t="n">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B11" t="n">
-        <v>90</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B12" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B14" t="n">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B15" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B16" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B18" t="n">
-        <v>99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B20" t="n">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="B21" t="n">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B22" t="n">
-        <v>79</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B23" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B24" t="n">
-        <v>97</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B25" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B26" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="B27" t="n">
-        <v>31</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B29" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B30" t="n">
-        <v>82</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B31" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B32" t="n">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B33" t="n">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B34" t="n">
         <v>95</v>
@@ -2103,42 +2438,194 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="B35" t="n">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B36" t="n">
-        <v>82</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B37" t="n">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B38" t="n">
-        <v>96</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B39" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>45</v>
+      </c>
+      <c r="B40" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>89</v>
+      </c>
+      <c r="B41" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>48</v>
+      </c>
+      <c r="B43" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>47</v>
+      </c>
+      <c r="B44" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>41</v>
+      </c>
+      <c r="B45" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>41</v>
+      </c>
+      <c r="B46" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>58</v>
+      </c>
+      <c r="B47" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>88</v>
+      </c>
+      <c r="B48" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>61</v>
+      </c>
+      <c r="B49" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>42</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>28</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>44</v>
+      </c>
+      <c r="B52" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>64</v>
+      </c>
+      <c r="B53" t="n">
         <v>92</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>66</v>
+      </c>
+      <c r="B54" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>64</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>50</v>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>97</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>95</v>
+      </c>
+      <c r="B58" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2146,7 +2633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2658,597 +3145,6 @@
       </c>
       <c r="B62" t="n">
         <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B71"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>95</v>
-      </c>
-      <c r="B3" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>62</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>63</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>91</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>45</v>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>65</v>
-      </c>
-      <c r="B8" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>32</v>
-      </c>
-      <c r="B9" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>46</v>
-      </c>
-      <c r="B10" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>54</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>62</v>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>56</v>
-      </c>
-      <c r="B13" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>70</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>70</v>
-      </c>
-      <c r="B15" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>63</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>64</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>68</v>
-      </c>
-      <c r="B18" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>63</v>
-      </c>
-      <c r="B19" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>83</v>
-      </c>
-      <c r="B20" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>85</v>
-      </c>
-      <c r="B21" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>85</v>
-      </c>
-      <c r="B22" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>59</v>
-      </c>
-      <c r="B23" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>59</v>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>58</v>
-      </c>
-      <c r="B25" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>50</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>53</v>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>53</v>
-      </c>
-      <c r="B28" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>86</v>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>73</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>74</v>
-      </c>
-      <c r="B31" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>74</v>
-      </c>
-      <c r="B32" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>89</v>
-      </c>
-      <c r="B33" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>94</v>
-      </c>
-      <c r="B34" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>90</v>
-      </c>
-      <c r="B35" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>44</v>
-      </c>
-      <c r="B36" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>92</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>86</v>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>98</v>
-      </c>
-      <c r="B39" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>45</v>
-      </c>
-      <c r="B40" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>80</v>
-      </c>
-      <c r="B41" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>84</v>
-      </c>
-      <c r="B42" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>78</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>71</v>
-      </c>
-      <c r="B44" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>27</v>
-      </c>
-      <c r="B45" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>39</v>
-      </c>
-      <c r="B46" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>75</v>
-      </c>
-      <c r="B47" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>87</v>
-      </c>
-      <c r="B48" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>41</v>
-      </c>
-      <c r="B49" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>70</v>
-      </c>
-      <c r="B51" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>55</v>
-      </c>
-      <c r="B52" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>30</v>
-      </c>
-      <c r="B53" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>56</v>
-      </c>
-      <c r="B54" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>57</v>
-      </c>
-      <c r="B55" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>57</v>
-      </c>
-      <c r="B56" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>92</v>
-      </c>
-      <c r="B57" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>96</v>
-      </c>
-      <c r="B58" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>76</v>
-      </c>
-      <c r="B59" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>76</v>
-      </c>
-      <c r="B60" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>73</v>
-      </c>
-      <c r="B61" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>58</v>
-      </c>
-      <c r="B62" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>55</v>
-      </c>
-      <c r="B63" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>28</v>
-      </c>
-      <c r="B64" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>27</v>
-      </c>
-      <c r="B65" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>30</v>
-      </c>
-      <c r="B66" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>12</v>
-      </c>
-      <c r="B67" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>12</v>
-      </c>
-      <c r="B68" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>84</v>
-      </c>
-      <c r="B69" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>47</v>
-      </c>
-      <c r="B70" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>9</v>
-      </c>
-      <c r="B71" t="n">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3485,7 +3381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3507,50 +3403,50 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>49</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B6" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B7" t="n">
-        <v>93</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -3558,255 +3454,255 @@
         <v>65</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="B10" t="n">
-        <v>60</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B11" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="B12" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B13" t="n">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B14" t="n">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B15" t="n">
-        <v>67</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B16" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B17" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B18" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B20" t="n">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" t="n">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B22" t="n">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B23" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B26" t="n">
-        <v>95</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B27" t="n">
-        <v>79</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B28" t="n">
-        <v>96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B29" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B30" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B31" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B32" t="n">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B33" t="n">
-        <v>93</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="B34" t="n">
-        <v>95</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B35" t="n">
-        <v>62</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="B38" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B39" t="n">
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -3814,151 +3710,255 @@
         <v>45</v>
       </c>
       <c r="B40" t="n">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B41" t="n">
-        <v>68</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="B42" t="n">
-        <v>58</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B43" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B44" t="n">
-        <v>67</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B45" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B47" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B49" t="n">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B52" t="n">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="B53" t="n">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B54" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B55" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>76</v>
+      </c>
+      <c r="B59" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>76</v>
+      </c>
+      <c r="B60" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>73</v>
+      </c>
+      <c r="B61" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>58</v>
+      </c>
+      <c r="B62" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>55</v>
+      </c>
+      <c r="B63" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>28</v>
+      </c>
+      <c r="B64" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>27</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30</v>
+      </c>
+      <c r="B66" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>12</v>
+      </c>
+      <c r="B67" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>12</v>
+      </c>
+      <c r="B68" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>84</v>
+      </c>
+      <c r="B69" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>47</v>
+      </c>
+      <c r="B70" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>9</v>
+      </c>
+      <c r="B71" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3967,6 +3967,1027 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>52</v>
+      </c>
+      <c r="B2" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B3" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>62</v>
+      </c>
+      <c r="B4" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>61</v>
+      </c>
+      <c r="B5" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B6" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33</v>
+      </c>
+      <c r="B7" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>65</v>
+      </c>
+      <c r="B8" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>48</v>
+      </c>
+      <c r="B9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>42</v>
+      </c>
+      <c r="B10" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>49</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>51</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>87</v>
+      </c>
+      <c r="B13" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>43</v>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>90</v>
+      </c>
+      <c r="B15" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>91</v>
+      </c>
+      <c r="B16" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>63</v>
+      </c>
+      <c r="B17" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>67</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>75</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>55</v>
+      </c>
+      <c r="B20" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>66</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>31</v>
+      </c>
+      <c r="B22" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>31</v>
+      </c>
+      <c r="B23" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>68</v>
+      </c>
+      <c r="B24" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>67</v>
+      </c>
+      <c r="B25" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>70</v>
+      </c>
+      <c r="B26" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>92</v>
+      </c>
+      <c r="B27" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>24</v>
+      </c>
+      <c r="B28" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>91</v>
+      </c>
+      <c r="B30" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>91</v>
+      </c>
+      <c r="B31" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>61</v>
+      </c>
+      <c r="B32" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>61</v>
+      </c>
+      <c r="B33" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>62</v>
+      </c>
+      <c r="B34" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>43</v>
+      </c>
+      <c r="B35" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>67</v>
+      </c>
+      <c r="B36" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>65</v>
+      </c>
+      <c r="B37" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>71</v>
+      </c>
+      <c r="B38" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>71</v>
+      </c>
+      <c r="B39" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>28</v>
+      </c>
+      <c r="B40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>43</v>
+      </c>
+      <c r="B41" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>53</v>
+      </c>
+      <c r="B42" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>75</v>
+      </c>
+      <c r="B43" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+      <c r="B44" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>59</v>
+      </c>
+      <c r="B45" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>52</v>
+      </c>
+      <c r="B46" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>43</v>
+      </c>
+      <c r="B47" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>63</v>
+      </c>
+      <c r="B48" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>97</v>
+      </c>
+      <c r="B49" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>68</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>43</v>
+      </c>
+      <c r="B51" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>46</v>
+      </c>
+      <c r="B52" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>35</v>
+      </c>
+      <c r="B53" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>35</v>
+      </c>
+      <c r="B54" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>43</v>
+      </c>
+      <c r="B55" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>38</v>
+      </c>
+      <c r="B56" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>28</v>
+      </c>
+      <c r="B57" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>33</v>
+      </c>
+      <c r="B58" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>27</v>
+      </c>
+      <c r="B59" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>61</v>
+      </c>
+      <c r="B60" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>75</v>
+      </c>
+      <c r="B61" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>40</v>
+      </c>
+      <c r="B62" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>40</v>
+      </c>
+      <c r="B63" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>56</v>
+      </c>
+      <c r="B64" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>43</v>
+      </c>
+      <c r="B65" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2" t="n">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B2" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>95</v>
+      </c>
+      <c r="B4" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>43</v>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>95</v>
+      </c>
+      <c r="B7" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>60</v>
+      </c>
+      <c r="B8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>45</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B10" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>52</v>
+      </c>
+      <c r="B12" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>77</v>
+      </c>
+      <c r="B13" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>38</v>
+      </c>
+      <c r="B14" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>50</v>
+      </c>
+      <c r="B15" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>50</v>
+      </c>
+      <c r="B16" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>29</v>
+      </c>
+      <c r="B17" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>40</v>
+      </c>
+      <c r="B18" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>35</v>
+      </c>
+      <c r="B19" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>58</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>63</v>
+      </c>
+      <c r="B21" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>58</v>
+      </c>
+      <c r="B22" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>58</v>
+      </c>
+      <c r="B23" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>58</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>48</v>
+      </c>
+      <c r="B25" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>94</v>
+      </c>
+      <c r="B26" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>92</v>
+      </c>
+      <c r="B27" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>92</v>
+      </c>
+      <c r="B28" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>93</v>
+      </c>
+      <c r="B29" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>40</v>
+      </c>
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>62</v>
+      </c>
+      <c r="B31" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>61</v>
+      </c>
+      <c r="B32" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>61</v>
+      </c>
+      <c r="B33" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>60</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>81</v>
+      </c>
+      <c r="B35" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>53</v>
+      </c>
+      <c r="B36" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>47</v>
+      </c>
+      <c r="B37" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>55</v>
+      </c>
+      <c r="B38" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>36</v>
+      </c>
+      <c r="B39" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>62</v>
+      </c>
+      <c r="B40" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>29</v>
+      </c>
+      <c r="B41" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>29</v>
+      </c>
+      <c r="B42" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>58</v>
+      </c>
+      <c r="B43" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>53</v>
+      </c>
+      <c r="B44" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>66</v>
+      </c>
+      <c r="B46" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>76</v>
+      </c>
+      <c r="B47" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>37</v>
+      </c>
+      <c r="B48" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>59</v>
+      </c>
+      <c r="B49" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>69</v>
+      </c>
+      <c r="B50" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>28</v>
+      </c>
+      <c r="B51" t="n">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4699,1025 +5720,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B66"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>52</v>
-      </c>
-      <c r="B2" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>59</v>
-      </c>
-      <c r="B3" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>62</v>
-      </c>
-      <c r="B4" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>61</v>
-      </c>
-      <c r="B5" t="n">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>63</v>
-      </c>
-      <c r="B6" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>33</v>
-      </c>
-      <c r="B7" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>65</v>
-      </c>
-      <c r="B8" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>48</v>
-      </c>
-      <c r="B9" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>42</v>
-      </c>
-      <c r="B10" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>49</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>51</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>87</v>
-      </c>
-      <c r="B13" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>43</v>
-      </c>
-      <c r="B14" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>90</v>
-      </c>
-      <c r="B15" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>91</v>
-      </c>
-      <c r="B16" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>63</v>
-      </c>
-      <c r="B17" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>67</v>
-      </c>
-      <c r="B18" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>75</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>55</v>
-      </c>
-      <c r="B20" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>66</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>31</v>
-      </c>
-      <c r="B22" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>31</v>
-      </c>
-      <c r="B23" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>68</v>
-      </c>
-      <c r="B24" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>67</v>
-      </c>
-      <c r="B25" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>70</v>
-      </c>
-      <c r="B26" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>92</v>
-      </c>
-      <c r="B27" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>24</v>
-      </c>
-      <c r="B28" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>91</v>
-      </c>
-      <c r="B30" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>91</v>
-      </c>
-      <c r="B31" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>61</v>
-      </c>
-      <c r="B32" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>61</v>
-      </c>
-      <c r="B33" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>62</v>
-      </c>
-      <c r="B34" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>43</v>
-      </c>
-      <c r="B35" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>67</v>
-      </c>
-      <c r="B36" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>65</v>
-      </c>
-      <c r="B37" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>71</v>
-      </c>
-      <c r="B38" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>71</v>
-      </c>
-      <c r="B39" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>28</v>
-      </c>
-      <c r="B40" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>43</v>
-      </c>
-      <c r="B41" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>53</v>
-      </c>
-      <c r="B42" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>75</v>
-      </c>
-      <c r="B43" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>44</v>
-      </c>
-      <c r="B44" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>59</v>
-      </c>
-      <c r="B45" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>52</v>
-      </c>
-      <c r="B46" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>43</v>
-      </c>
-      <c r="B47" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>63</v>
-      </c>
-      <c r="B48" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>97</v>
-      </c>
-      <c r="B49" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>68</v>
-      </c>
-      <c r="B50" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>43</v>
-      </c>
-      <c r="B51" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>46</v>
-      </c>
-      <c r="B52" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>35</v>
-      </c>
-      <c r="B53" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>35</v>
-      </c>
-      <c r="B54" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>43</v>
-      </c>
-      <c r="B55" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>38</v>
-      </c>
-      <c r="B56" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>28</v>
-      </c>
-      <c r="B57" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>33</v>
-      </c>
-      <c r="B58" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>27</v>
-      </c>
-      <c r="B59" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>61</v>
-      </c>
-      <c r="B60" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>75</v>
-      </c>
-      <c r="B61" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>40</v>
-      </c>
-      <c r="B62" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>40</v>
-      </c>
-      <c r="B63" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>56</v>
-      </c>
-      <c r="B64" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>43</v>
-      </c>
-      <c r="B65" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" t="n">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B2" t="n">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>38</v>
-      </c>
-      <c r="B2" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>43</v>
-      </c>
-      <c r="B3" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>95</v>
-      </c>
-      <c r="B4" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>43</v>
-      </c>
-      <c r="B5" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>47</v>
-      </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>95</v>
-      </c>
-      <c r="B7" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>60</v>
-      </c>
-      <c r="B8" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>45</v>
-      </c>
-      <c r="B9" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>45</v>
-      </c>
-      <c r="B10" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>45</v>
-      </c>
-      <c r="B11" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>52</v>
-      </c>
-      <c r="B12" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>77</v>
-      </c>
-      <c r="B13" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>38</v>
-      </c>
-      <c r="B14" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>50</v>
-      </c>
-      <c r="B15" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>50</v>
-      </c>
-      <c r="B16" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>29</v>
-      </c>
-      <c r="B17" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>40</v>
-      </c>
-      <c r="B18" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>35</v>
-      </c>
-      <c r="B19" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>58</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>63</v>
-      </c>
-      <c r="B21" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>58</v>
-      </c>
-      <c r="B22" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>58</v>
-      </c>
-      <c r="B23" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>58</v>
-      </c>
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>48</v>
-      </c>
-      <c r="B25" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>94</v>
-      </c>
-      <c r="B26" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>92</v>
-      </c>
-      <c r="B27" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>92</v>
-      </c>
-      <c r="B28" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>93</v>
-      </c>
-      <c r="B29" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>40</v>
-      </c>
-      <c r="B30" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>62</v>
-      </c>
-      <c r="B31" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>61</v>
-      </c>
-      <c r="B32" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>61</v>
-      </c>
-      <c r="B33" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>60</v>
-      </c>
-      <c r="B34" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>81</v>
-      </c>
-      <c r="B35" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>53</v>
-      </c>
-      <c r="B36" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>47</v>
-      </c>
-      <c r="B37" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>55</v>
-      </c>
-      <c r="B38" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>36</v>
-      </c>
-      <c r="B39" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>62</v>
-      </c>
-      <c r="B40" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>29</v>
-      </c>
-      <c r="B41" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>29</v>
-      </c>
-      <c r="B42" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>58</v>
-      </c>
-      <c r="B43" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>53</v>
-      </c>
-      <c r="B44" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>66</v>
-      </c>
-      <c r="B46" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>76</v>
-      </c>
-      <c r="B47" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>37</v>
-      </c>
-      <c r="B48" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>59</v>
-      </c>
-      <c r="B49" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>69</v>
-      </c>
-      <c r="B50" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>28</v>
-      </c>
-      <c r="B51" t="n">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>